<commit_message>
juan Carlos and Andre´s parts
</commit_message>
<xml_diff>
--- a/backlogCVcreator.xlsx
+++ b/backlogCVcreator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albc8\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B577EBF-7C1C-466E-B0CF-0182A5130F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A055E7A-E444-490C-B531-BE88D3226257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2030" yWindow="1580" windowWidth="19200" windowHeight="11170" tabRatio="833" firstSheet="6" activeTab="12" xr2:uid="{719016E5-AE26-4BAA-BABB-F43F55BF4197}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="833" firstSheet="21" activeTab="26" xr2:uid="{719016E5-AE26-4BAA-BABB-F43F55BF4197}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="221">
   <si>
     <t>1. Planificación</t>
   </si>
@@ -358,9 +358,6 @@
   </si>
   <si>
     <t>Despliegue</t>
-  </si>
-  <si>
-    <t>Producción</t>
   </si>
   <si>
     <t>Crear documentación</t>
@@ -660,6 +657,84 @@
   </si>
   <si>
     <t>Activación de botón de descarga en la UI</t>
+  </si>
+  <si>
+    <t>Analista funcional</t>
+  </si>
+  <si>
+    <t>Generación de la documentación técnica y funcional del sistema web</t>
+  </si>
+  <si>
+    <t>La documentación debe estar completa, clara y actualizada.</t>
+  </si>
+  <si>
+    <t>Documento PDF/Word de la documentación técnica y funcional.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema web ha sido terminado en su priomera version </t>
+  </si>
+  <si>
+    <t>1 Analista funcional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 días hábiles </t>
+  </si>
+  <si>
+    <t>Recolección de información</t>
+  </si>
+  <si>
+    <t>Redacción inicial</t>
+  </si>
+  <si>
+    <t>Actividad destinada a identificar vulnerabilidades en el sistema web mediante pruebas de seguridad,</t>
+  </si>
+  <si>
+    <t>No deben encontrarse vulnerabilidades críticas o altas.</t>
+  </si>
+  <si>
+    <t>Checklist de cumplimiento de buenas prácticas (OWASP).</t>
+  </si>
+  <si>
+    <t>El sistema está en un entorno estable o de staging para pruebas.</t>
+  </si>
+  <si>
+    <t>1 Especialista en ciberseguridad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 días hábiles </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preparación y configuración del entorno de prueba </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documentación de resultados y recomendaciones </t>
+  </si>
+  <si>
+    <t>Desarrollo y ejecución de pruebas unitarias para validar el correcto funcionamiento de componentes</t>
+  </si>
+  <si>
+    <t>Cobertura mínima del 80% de los módulos críticos.</t>
+  </si>
+  <si>
+    <t>Código fuente de pruebas unitarias.</t>
+  </si>
+  <si>
+    <t>El sistema tiene una arquitectura modular que permite pruebas unitarias.</t>
+  </si>
+  <si>
+    <t>2 Desarrolladores (frontend y backend) y 1 QA (para validación de casos cubiertos)</t>
+  </si>
+  <si>
+    <t>4 días hábiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identificación de componentes a testear </t>
+  </si>
+  <si>
+    <t>Implementación de pruebas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	$ 880</t>
   </si>
 </sst>
 </file>
@@ -667,7 +742,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -882,7 +957,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -916,26 +991,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -952,6 +1010,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -6286,9 +6359,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6326,7 +6399,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -6432,7 +6505,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6574,7 +6647,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6588,176 +6661,176 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -6776,19 +6849,19 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB009B5F-CFA5-40C7-B7C8-CBDD8E6B383C}">
-  <dimension ref="A2:O18"/>
+  <dimension ref="A2:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" customWidth="1"/>
-    <col min="8" max="8" width="16.90625" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -6814,7 +6887,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>9</v>
       </c>
@@ -6838,29 +6911,29 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B7" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -6871,17 +6944,13 @@
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-    </row>
-    <row r="9" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -6893,12 +6962,12 @@
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
     </row>
-    <row r="10" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -6910,12 +6979,12 @@
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
     </row>
-    <row r="11" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -6927,12 +6996,12 @@
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -6944,12 +7013,12 @@
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -6961,37 +7030,37 @@
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="28"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="21"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="23">
+      <c r="B15" s="16">
         <v>400</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="25"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="18"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -7001,15 +7070,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="B8:K8"/>
+    <mergeCell ref="B9:K9"/>
+    <mergeCell ref="B10:K10"/>
     <mergeCell ref="B11:K11"/>
     <mergeCell ref="B12:K12"/>
     <mergeCell ref="B13:K13"/>
     <mergeCell ref="B15:K15"/>
     <mergeCell ref="B14:K14"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="B8:K8"/>
-    <mergeCell ref="B9:K9"/>
-    <mergeCell ref="B10:K10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7024,13 +7093,13 @@
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.90625" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -7056,7 +7125,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>10</v>
       </c>
@@ -7080,12 +7149,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -7094,12 +7163,12 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -7108,12 +7177,12 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -7122,12 +7191,12 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -7136,12 +7205,12 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -7150,12 +7219,12 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -7164,12 +7233,12 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -7178,7 +7247,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -7188,7 +7257,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
@@ -7202,7 +7271,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -7229,19 +7298,19 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F1F8BFA-32B2-45F8-8A47-5FBDD6265581}">
-  <dimension ref="A2:I18"/>
+  <dimension ref="A2:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="8" max="8" width="16.54296875" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -7267,7 +7336,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>11</v>
       </c>
@@ -7291,41 +7360,40 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="22"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B7" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="21" t="s">
-        <v>183</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B8" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -7334,12 +7402,12 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -7348,12 +7416,12 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -7362,7 +7430,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
@@ -7376,12 +7444,12 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -7390,10 +7458,10 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -7402,7 +7470,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
@@ -7416,7 +7484,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -7445,16 +7513,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FA33F1-5BDE-4D44-8A9A-B5CD2ECCA57D}">
   <dimension ref="A2:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -7480,7 +7548,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>12</v>
       </c>
@@ -7504,138 +7572,138 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
+      <c r="B7" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="30" t="s">
-        <v>191</v>
-      </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="29"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B8" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="27"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="29"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B9" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="27"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="29"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B10" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="27"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="29"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B11" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="27"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="29"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B12" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="27"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="29"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B13" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="27"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="29"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B14" s="23"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="27"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="23">
         <v>500</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="29"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="27"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -7667,9 +7735,9 @@
       <selection activeCell="B15" sqref="B15:H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -7695,7 +7763,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>13</v>
       </c>
@@ -7719,12 +7787,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -7733,12 +7801,12 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -7747,12 +7815,12 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -7761,12 +7829,12 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -7775,12 +7843,12 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -7789,12 +7857,12 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -7803,12 +7871,12 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -7817,10 +7885,10 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -7829,12 +7897,12 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -7843,7 +7911,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -7876,9 +7944,9 @@
       <selection activeCell="B15" sqref="B15:H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -7904,7 +7972,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>14</v>
       </c>
@@ -7928,12 +7996,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -7942,12 +8010,12 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -7956,12 +8024,12 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -7970,12 +8038,12 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -7984,12 +8052,12 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -7998,12 +8066,12 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -8012,12 +8080,12 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -8026,10 +8094,10 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -8038,12 +8106,12 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -8052,7 +8120,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -8085,9 +8153,9 @@
       <selection activeCell="B8" sqref="B8:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -8113,7 +8181,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>15</v>
       </c>
@@ -8137,7 +8205,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
@@ -8149,7 +8217,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
@@ -8161,7 +8229,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
@@ -8173,7 +8241,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
@@ -8185,7 +8253,7 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
@@ -8197,7 +8265,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
@@ -8209,7 +8277,7 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
@@ -8221,7 +8289,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -8231,7 +8299,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
@@ -8243,7 +8311,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -8276,9 +8344,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -8304,7 +8372,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>16</v>
       </c>
@@ -8328,7 +8396,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
@@ -8340,7 +8408,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
@@ -8352,7 +8420,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
@@ -8364,7 +8432,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
@@ -8376,7 +8444,7 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
@@ -8388,7 +8456,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
@@ -8400,7 +8468,7 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
@@ -8412,7 +8480,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -8422,7 +8490,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
@@ -8434,7 +8502,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -8467,9 +8535,9 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -8495,7 +8563,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>17</v>
       </c>
@@ -8519,7 +8587,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
@@ -8531,7 +8599,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
@@ -8543,7 +8611,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
@@ -8555,7 +8623,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
@@ -8567,7 +8635,7 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
@@ -8579,7 +8647,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
@@ -8591,7 +8659,7 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
@@ -8603,7 +8671,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -8613,7 +8681,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
@@ -8625,7 +8693,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -8658,9 +8726,9 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -8686,7 +8754,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>18</v>
       </c>
@@ -8710,7 +8778,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
@@ -8722,7 +8790,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
@@ -8734,7 +8802,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
@@ -8746,7 +8814,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
@@ -8758,7 +8826,7 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
@@ -8770,7 +8838,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
@@ -8782,7 +8850,7 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
@@ -8794,7 +8862,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -8804,7 +8872,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
@@ -8816,7 +8884,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -8849,15 +8917,15 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" customWidth="1"/>
-    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -8883,7 +8951,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>62</v>
       </c>
@@ -8913,17 +8981,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
@@ -8937,7 +9005,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
@@ -8951,7 +9019,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
@@ -8965,7 +9033,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
@@ -8979,7 +9047,7 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
@@ -8993,7 +9061,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
@@ -9007,7 +9075,7 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
@@ -9021,7 +9089,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13" t="s">
         <v>60</v>
@@ -9033,7 +9101,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
@@ -9047,7 +9115,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -9055,7 +9123,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
@@ -9085,9 +9153,9 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -9113,7 +9181,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>19</v>
       </c>
@@ -9137,7 +9205,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
@@ -9149,7 +9217,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
@@ -9161,7 +9229,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
@@ -9173,7 +9241,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
@@ -9185,7 +9253,7 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
@@ -9197,7 +9265,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
@@ -9209,7 +9277,7 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
@@ -9221,7 +9289,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -9231,7 +9299,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
@@ -9243,7 +9311,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -9276,9 +9344,9 @@
       <selection activeCell="B7" sqref="B7:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -9304,7 +9372,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>20</v>
       </c>
@@ -9328,7 +9396,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
@@ -9340,7 +9408,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
@@ -9352,7 +9420,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
@@ -9364,7 +9432,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
@@ -9376,7 +9444,7 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
@@ -9388,7 +9456,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
@@ -9400,7 +9468,7 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
@@ -9412,7 +9480,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -9422,7 +9490,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
@@ -9434,7 +9502,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -9467,9 +9535,9 @@
       <selection activeCell="B15" sqref="B15:H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -9495,7 +9563,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>21</v>
       </c>
@@ -9519,7 +9587,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
@@ -9531,7 +9599,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
@@ -9543,7 +9611,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
@@ -9555,7 +9623,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
@@ -9567,7 +9635,7 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
@@ -9579,7 +9647,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
@@ -9591,7 +9659,7 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
@@ -9603,7 +9671,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -9613,7 +9681,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
@@ -9625,7 +9693,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -9658,9 +9726,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -9686,7 +9754,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>22</v>
       </c>
@@ -9710,7 +9778,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
@@ -9722,7 +9790,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
@@ -9734,7 +9802,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
@@ -9746,7 +9814,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
@@ -9758,7 +9826,7 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
@@ -9770,7 +9838,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
@@ -9782,7 +9850,7 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
@@ -9794,7 +9862,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -9804,7 +9872,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
@@ -9816,7 +9884,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -9849,9 +9917,9 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -9877,7 +9945,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>23</v>
       </c>
@@ -9901,7 +9969,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
@@ -9913,7 +9981,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
@@ -9925,7 +9993,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
@@ -9937,7 +10005,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
@@ -9949,7 +10017,7 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
@@ -9961,7 +10029,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
@@ -9973,7 +10041,7 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
@@ -9985,7 +10053,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -9995,7 +10063,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
@@ -10007,7 +10075,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -10040,9 +10108,9 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -10068,7 +10136,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>24</v>
       </c>
@@ -10092,7 +10160,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
@@ -10104,7 +10172,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
@@ -10116,7 +10184,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
@@ -10128,7 +10196,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
@@ -10140,7 +10208,7 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
@@ -10152,7 +10220,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
@@ -10164,7 +10232,7 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
@@ -10176,7 +10244,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -10186,7 +10254,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
@@ -10198,7 +10266,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -10231,9 +10299,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -10259,7 +10327,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>25</v>
       </c>
@@ -10283,7 +10351,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
@@ -10295,7 +10363,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
@@ -10307,7 +10375,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
@@ -10319,7 +10387,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
@@ -10331,7 +10399,7 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
@@ -10343,7 +10411,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
@@ -10355,7 +10423,7 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
@@ -10367,7 +10435,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -10377,7 +10445,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
@@ -10389,7 +10457,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -10418,13 +10486,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8861A054-7840-4778-8D64-92E726F35744}">
   <dimension ref="A2:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -10450,15 +10518,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>93</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D3" s="4">
         <v>45811</v>
@@ -10474,11 +10542,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="13" t="s">
+        <v>212</v>
+      </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -10486,11 +10556,13 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="13"/>
+      <c r="B8" s="13" t="s">
+        <v>213</v>
+      </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
@@ -10498,11 +10570,13 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="13"/>
+      <c r="B9" s="13" t="s">
+        <v>214</v>
+      </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -10510,11 +10584,13 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="13"/>
+      <c r="B10" s="13" t="s">
+        <v>215</v>
+      </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -10522,11 +10598,13 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="13"/>
+      <c r="B11" s="14" t="s">
+        <v>216</v>
+      </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
@@ -10534,11 +10612,13 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="13"/>
+      <c r="B12" s="13" t="s">
+        <v>217</v>
+      </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
@@ -10546,11 +10626,13 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="13" t="s">
+        <v>218</v>
+      </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
@@ -10558,9 +10640,11 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="13"/>
+      <c r="B14" s="13" t="s">
+        <v>219</v>
+      </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
@@ -10568,11 +10652,13 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="13"/>
+      <c r="B15" s="13" t="s">
+        <v>220</v>
+      </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
@@ -10580,7 +10666,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -10609,13 +10695,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79921DD6-F724-4577-93F4-D76CE0DD6CD9}">
   <dimension ref="A2:H18"/>
   <sheetViews>
-    <sheetView topLeftCell="E3" workbookViewId="0">
-      <selection sqref="A1:H19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -10641,15 +10727,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D3" s="4">
         <v>45811</v>
@@ -10665,11 +10751,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="13" t="s">
+        <v>204</v>
+      </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -10677,11 +10765,13 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="13"/>
+      <c r="B8" s="13" t="s">
+        <v>205</v>
+      </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
@@ -10689,11 +10779,13 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="13"/>
+      <c r="B9" s="13" t="s">
+        <v>206</v>
+      </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -10701,11 +10793,13 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="13"/>
+      <c r="B10" s="13" t="s">
+        <v>207</v>
+      </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -10713,11 +10807,13 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="13"/>
+      <c r="B11" s="13" t="s">
+        <v>208</v>
+      </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
@@ -10725,11 +10821,13 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="13"/>
+      <c r="B12" s="13" t="s">
+        <v>209</v>
+      </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
@@ -10737,11 +10835,13 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="13" t="s">
+        <v>210</v>
+      </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
@@ -10749,9 +10849,11 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="13"/>
+      <c r="B14" s="13" t="s">
+        <v>211</v>
+      </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
@@ -10759,11 +10861,13 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="13"/>
+      <c r="B15" s="15">
+        <v>1360</v>
+      </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
@@ -10771,7 +10875,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -10801,12 +10905,12 @@
   <dimension ref="A2:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection sqref="A1:H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -10832,7 +10936,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>28</v>
       </c>
@@ -10840,12 +10944,14 @@
         <v>97</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D3" s="4">
         <v>45811</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>195</v>
+      </c>
       <c r="F3" s="4">
         <v>45796</v>
       </c>
@@ -10856,11 +10962,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="13" t="s">
+        <v>196</v>
+      </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -10868,11 +10976,13 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="13"/>
+      <c r="B8" s="13" t="s">
+        <v>197</v>
+      </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
@@ -10880,11 +10990,13 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="13"/>
+      <c r="B9" s="13" t="s">
+        <v>198</v>
+      </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -10892,11 +11004,13 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="13"/>
+      <c r="B10" s="13" t="s">
+        <v>199</v>
+      </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -10904,11 +11018,13 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="13"/>
+      <c r="B11" s="13" t="s">
+        <v>200</v>
+      </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
@@ -10916,11 +11032,13 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="13"/>
+      <c r="B12" s="13" t="s">
+        <v>201</v>
+      </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
@@ -10928,11 +11046,13 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="13" t="s">
+        <v>202</v>
+      </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
@@ -10940,9 +11060,11 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="13"/>
+      <c r="B14" s="13" t="s">
+        <v>203</v>
+      </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
@@ -10950,11 +11072,13 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="13"/>
+      <c r="B15" s="15">
+        <v>630</v>
+      </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
@@ -10962,7 +11086,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -10995,12 +11119,12 @@
       <selection activeCell="B11" sqref="B11:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -11026,7 +11150,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -11055,17 +11179,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
@@ -11079,7 +11203,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
@@ -11093,7 +11217,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
@@ -11107,12 +11231,12 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -11121,7 +11245,7 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
@@ -11135,7 +11259,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
@@ -11149,7 +11273,7 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
@@ -11163,7 +11287,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13" t="s">
         <v>70</v>
@@ -11175,7 +11299,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
@@ -11189,7 +11313,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -11222,16 +11346,16 @@
       <selection activeCell="B8" sqref="B8:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.26953125" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" customWidth="1"/>
-    <col min="3" max="3" width="26.7265625" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -11257,7 +11381,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>3</v>
       </c>
@@ -11271,7 +11395,7 @@
         <v>45811</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F3" s="4">
         <v>45796</v>
@@ -11283,12 +11407,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -11297,12 +11421,12 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -11311,12 +11435,12 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -11325,12 +11449,12 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -11339,7 +11463,7 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
@@ -11353,12 +11477,12 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -11367,12 +11491,12 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -11381,10 +11505,10 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -11393,12 +11517,12 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -11407,7 +11531,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -11440,15 +11564,15 @@
       <selection activeCell="B15" sqref="B15:H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" customWidth="1"/>
-    <col min="3" max="3" width="19.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -11474,7 +11598,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>4</v>
       </c>
@@ -11498,12 +11622,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -11512,12 +11636,12 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -11526,12 +11650,12 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -11540,12 +11664,12 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -11554,12 +11678,12 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -11568,12 +11692,12 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -11582,12 +11706,12 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -11596,10 +11720,10 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -11608,12 +11732,12 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -11622,7 +11746,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -11655,9 +11779,9 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -11683,7 +11807,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>5</v>
       </c>
@@ -11707,12 +11831,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -11721,12 +11845,12 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -11735,12 +11859,12 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -11749,12 +11873,12 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -11763,12 +11887,12 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -11777,12 +11901,12 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -11791,12 +11915,12 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -11805,10 +11929,10 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -11817,7 +11941,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
@@ -11831,7 +11955,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -11864,9 +11988,9 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -11892,7 +12016,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>6</v>
       </c>
@@ -11916,12 +12040,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -11930,12 +12054,12 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -11944,12 +12068,12 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -11958,12 +12082,12 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -11972,12 +12096,12 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -11986,12 +12110,12 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -12000,12 +12124,12 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -12014,10 +12138,10 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -12026,7 +12150,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
@@ -12040,7 +12164,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -12073,9 +12197,9 @@
       <selection activeCell="B15" sqref="B15:H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -12101,7 +12225,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>7</v>
       </c>
@@ -12125,12 +12249,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -12139,12 +12263,12 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -12153,12 +12277,12 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -12167,12 +12291,12 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -12181,12 +12305,12 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -12195,12 +12319,12 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -12209,12 +12333,12 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -12223,10 +12347,10 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -12235,12 +12359,12 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -12249,7 +12373,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -12282,9 +12406,9 @@
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -12310,7 +12434,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>8</v>
       </c>
@@ -12334,12 +12458,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -12348,12 +12472,12 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -12362,12 +12486,12 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -12376,12 +12500,12 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -12390,12 +12514,12 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -12404,12 +12528,12 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -12418,12 +12542,12 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -12432,10 +12556,10 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -12444,12 +12568,12 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -12458,7 +12582,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>

</xml_diff>